<commit_message>
add publication base file as excel
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuk/git-web/stsykw.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87F0F40-627E-1749-87C8-77C9E2F1931A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D5F1E-8017-EA4D-8841-CEEA80239B15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="24820" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1785,7 +1785,7 @@
   </sheetPr>
   <dimension ref="A1:IV72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1794,7 +1794,7 @@
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="78.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="50.42578125" style="1" customWidth="1"/>

</xml_diff>